<commit_message>
thêm import export sản phẩm bằng Excel
</commit_message>
<xml_diff>
--- a/App_View/wwwroot/excel/template.xlsx
+++ b/App_View/wwwroot/excel/template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27004"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_92480E3D80EBD8D2623DC6FA873E8C18510380D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B226AA-84BC-48C7-9084-F5D7DE072E24}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="11_92480E3D80EBD8D2623DC6FA873E8C18510380D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAEBADFD-1BF9-4503-8818-33F7BB21B948}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="54">
   <si>
     <t>Tên SP</t>
   </si>
@@ -75,32 +75,128 @@
     <t>Ảnh</t>
   </si>
   <si>
-    <t>Atrbuti</t>
+    <t>Running Shoes</t>
   </si>
   <si>
     <t>Adidas</t>
   </si>
   <si>
-    <t>Việt Nam</t>
-  </si>
-  <si>
-    <t>Vải</t>
-  </si>
-  <si>
-    <t>Giầy Adidas</t>
-  </si>
-  <si>
-    <t>Đế mềm</t>
-  </si>
-  <si>
-    <t>yellow</t>
+    <t>Đức</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>Giày chạy bộ</t>
+  </si>
+  <si>
+    <t>Đế đàn hồi</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>Duramo10_1.png,Duramo10_2.png,Duramo10_3.png,Duramo10_4.png</t>
+  </si>
+  <si>
+    <t>RIVALRY 86 LOW</t>
+  </si>
+  <si>
+    <t>Giày thể thao</t>
+  </si>
+  <si>
+    <t>Đế phẳng</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>RIVALRY1.png,RIVALRY2.png,RIVALRY3.png,RIVALRY4.png</t>
+  </si>
+  <si>
+    <t>DURAMO SPEED</t>
+  </si>
+  <si>
+    <t>Đế đinh</t>
+  </si>
+  <si>
+    <t>DURAMO_SPEED_black1.png,DURAMO_SPEED_black2.png,DURAMO_SPEED_black3.png,DURAMO_SPEED_black4.png</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>DURAMO_SPEED_blue1.png,DURAMO_SPEED_blue2.png,DURAMO_SPEED_blue3.png,DURAMO_SPEED_blue4.png</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>DURAMO_SPEED_green1.png,DURAMO_SPEED_green2.png,DURAMO_SPEED_green4.png</t>
+  </si>
+  <si>
+    <t>HEAWYN</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>HEAWYN1.png,HEAWYN2.png,HEAWYN3.png,HEAWYN4.png</t>
+  </si>
+  <si>
+    <t>GALAXY 6</t>
+  </si>
+  <si>
+    <t>Chạy</t>
+  </si>
+  <si>
+    <t>GALAXY6_1.png,GALAXY6_2.png,GALAXY6_3.png,GALAXY6_4.png</t>
+  </si>
+  <si>
+    <t>GALAXY6_blue1.png,GALAXY6_blue2.png,GALAXY6_blue3.png,GALAXY6_blue4.png</t>
+  </si>
+  <si>
+    <t>ADICROSS LOW</t>
+  </si>
+  <si>
+    <t>Đánh gold</t>
+  </si>
+  <si>
+    <t>ADICROSS_LOW_1.png,ADICROSS_LOW_2.png,ADICROSS_LOW_3.png,ADICROSS_LOW_4.png</t>
+  </si>
+  <si>
+    <t>RIVALRY LOW</t>
+  </si>
+  <si>
+    <t>RIVALRY_LOW1.png,RIVALRY_LOW2.png,RIVALRY_LOW3.png,RIVALRY_LOW4.png</t>
+  </si>
+  <si>
+    <t>Impact 4</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>Giày bóng rổ</t>
+  </si>
+  <si>
+    <t>Impact_4_1.png,Impact_4_2.png,Impact_4_3.png,Impact_4_4.png</t>
+  </si>
+  <si>
+    <t>Air Max SC Leather</t>
+  </si>
+  <si>
+    <t>Men's Shoes</t>
+  </si>
+  <si>
+    <t>Air_Max_SC_Leather1.png,Air_Max_SC_Leather2.png,Air_Max_SC_Leather3.png,Air_Max_SC_Leather4.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +211,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF111111"/>
+      <name val="Helvetica Now Text Medium"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -145,6 +253,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -459,27 +569,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="107.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75">
@@ -554,11 +664,11 @@
       <c r="H2" s="2">
         <v>32</v>
       </c>
-      <c r="I2" s="2">
-        <v>50000</v>
+      <c r="I2">
+        <v>2000000</v>
       </c>
       <c r="J2" s="2">
-        <v>60000</v>
+        <v>2100000</v>
       </c>
       <c r="K2" s="2">
         <v>500</v>
@@ -571,6 +681,526 @@
       </c>
       <c r="N2" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <v>31</v>
+      </c>
+      <c r="I3">
+        <v>2000000</v>
+      </c>
+      <c r="J3">
+        <v>2900000</v>
+      </c>
+      <c r="K3" s="2">
+        <v>500</v>
+      </c>
+      <c r="L3" s="2">
+        <v>500</v>
+      </c>
+      <c r="M3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>2400000</v>
+      </c>
+      <c r="J4">
+        <v>2500000</v>
+      </c>
+      <c r="K4">
+        <v>200</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5">
+        <v>31</v>
+      </c>
+      <c r="I5">
+        <v>2400000</v>
+      </c>
+      <c r="J5">
+        <v>2500000</v>
+      </c>
+      <c r="K5">
+        <v>200</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6">
+        <v>32</v>
+      </c>
+      <c r="I6">
+        <v>2400000</v>
+      </c>
+      <c r="J6">
+        <v>2500000</v>
+      </c>
+      <c r="K6">
+        <v>200</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <v>33</v>
+      </c>
+      <c r="I7">
+        <v>2400000</v>
+      </c>
+      <c r="J7">
+        <v>26000000</v>
+      </c>
+      <c r="K7">
+        <v>200</v>
+      </c>
+      <c r="L7">
+        <v>100</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8">
+        <v>33</v>
+      </c>
+      <c r="I8">
+        <v>2400000</v>
+      </c>
+      <c r="J8">
+        <v>26000000</v>
+      </c>
+      <c r="K8">
+        <v>200</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="18">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9">
+        <v>33</v>
+      </c>
+      <c r="I9">
+        <v>2400000</v>
+      </c>
+      <c r="J9">
+        <v>2700000</v>
+      </c>
+      <c r="K9">
+        <v>200</v>
+      </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10">
+        <v>33</v>
+      </c>
+      <c r="I10">
+        <v>2400000</v>
+      </c>
+      <c r="J10">
+        <v>28900000</v>
+      </c>
+      <c r="K10">
+        <v>200</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="18">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11">
+        <v>33</v>
+      </c>
+      <c r="I11">
+        <v>2400000</v>
+      </c>
+      <c r="J11">
+        <v>28900000</v>
+      </c>
+      <c r="K11">
+        <v>200</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="18">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12">
+        <v>33</v>
+      </c>
+      <c r="I12">
+        <v>2400000</v>
+      </c>
+      <c r="J12">
+        <v>28900000</v>
+      </c>
+      <c r="K12">
+        <v>200</v>
+      </c>
+      <c r="L12">
+        <v>100</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13">
+        <v>33</v>
+      </c>
+      <c r="I13">
+        <v>2400000</v>
+      </c>
+      <c r="J13">
+        <v>28900000</v>
+      </c>
+      <c r="K13">
+        <v>200</v>
+      </c>
+      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>